<commit_message>
Seleció dies, afegir Diners, selecionar infant,
</commit_message>
<xml_diff>
--- a/Documentació/Diagrama de gantt.xlsx
+++ b/Documentació/Diagrama de gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\OneDrive\Escritorio\TFG\Documentació\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05EA195-3E86-4438-B953-67CF4B082D39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCD806D-4CF9-4FA2-BA27-9E254550B72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1328705C-3769-49BC-8F2C-035A8F58077A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Semana 1</t>
   </si>
@@ -159,13 +160,16 @@
   </si>
   <si>
     <t>Presentació final</t>
+  </si>
+  <si>
+    <t>Veure tots els infants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,15 +178,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -255,20 +266,201 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,18 +775,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC060DA9-206D-4910-B4E3-F30BB8E1900E}">
-  <dimension ref="B4:U30"/>
+  <dimension ref="B2:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="24"/>
+    </row>
+    <row r="4" spans="2:21" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -654,14 +867,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -678,8 +891,8 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="3"/>
@@ -702,8 +915,8 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="1"/>
@@ -726,8 +939,8 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="1"/>
@@ -750,8 +963,8 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:21" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="1"/>
@@ -774,8 +987,8 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+    <row r="10" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="9"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -796,8 +1009,8 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="1"/>
@@ -820,14 +1033,14 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -844,15 +1057,15 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -868,16 +1081,16 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -892,81 +1105,81 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="2:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+    </row>
+    <row r="16" spans="2:21" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="23"/>
+    </row>
+    <row r="17" spans="2:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="B17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+    </row>
+    <row r="18" spans="2:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -974,9 +1187,9 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -988,9 +1201,9 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>29</v>
+    <row r="19" spans="2:21" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -999,8 +1212,8 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="8"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1012,9 +1225,9 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>33</v>
+    <row r="20" spans="2:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1024,9 +1237,9 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1036,9 +1249,9 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>37</v>
+    <row r="21" spans="2:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1049,8 +1262,8 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="8"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1060,9 +1273,9 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>34</v>
+    <row r="22" spans="2:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1074,9 +1287,9 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -1084,9 +1297,9 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>35</v>
+    <row r="23" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1099,72 +1312,74 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+    <row r="24" spans="2:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+    <row r="25" spans="2:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="8"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+    <row r="26" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1173,15 +1388,13 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="R26" s="5"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="27" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1196,15 +1409,15 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>40</v>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B28" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1220,15 +1433,15 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>41</v>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+    </row>
+    <row r="29" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B29" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1244,14 +1457,16 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B30" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1269,11 +1484,33 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="B31" s="9"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>